<commit_message>
usr mngmt error vldt
</commit_message>
<xml_diff>
--- a/USER_MANAGEMENET_ERR_VALIDATION/input_data/datapool/User_Management_Err_Validation.xlsx
+++ b/USER_MANAGEMENET_ERR_VALIDATION/input_data/datapool/User_Management_Err_Validation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4554512-0DB6-452A-AE90-27DE7F7D6289}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA409C8-8097-41A1-A4A7-B325DE61F46F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="582" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="582" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios" sheetId="15" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <definedName name="YesOrNo">dropdowns!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="346">
   <si>
     <t>Active</t>
   </si>
@@ -980,9 +981,6 @@
     <t>David.Roberts</t>
   </si>
   <si>
-    <t>David.Roberts@gmail.com</t>
-  </si>
-  <si>
     <t>Job Title is required!</t>
   </si>
   <si>
@@ -1026,13 +1024,79 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>DaviddavidDaviddavidDaviddavidDaviddavidDaviddavidDaviddavidBigger</t>
+  </si>
+  <si>
+    <t>RobertsRobertsRobertsRobertsRobertsRobertsRobertsRobertsRobertsBigger</t>
+  </si>
+  <si>
+    <t>David.Roberts@militsdev.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>David Roberts@militsdev.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>hmouloud1@gmail.com</t>
+  </si>
+  <si>
+    <t>JobTitleJobTitleJobTitleJobTitleJobTitleJobTitleJobTitleJobTitleBigger</t>
+  </si>
+  <si>
+    <t>Job Title cannot contain special characters and must be less than 64 characters.</t>
+  </si>
+  <si>
+    <t>Job ##</t>
+  </si>
+  <si>
+    <t>Job 123</t>
+  </si>
+  <si>
+    <t>Employee Type is required!</t>
+  </si>
+  <si>
+    <t>Contractor</t>
+  </si>
+  <si>
+    <t>Validate_User_Office</t>
+  </si>
+  <si>
+    <t>Carrington Metuge</t>
+  </si>
+  <si>
+    <t>ADCVD Office I</t>
+  </si>
+  <si>
+    <t>Validate_User_Manager</t>
+  </si>
+  <si>
+    <t>Office is required</t>
+  </si>
+  <si>
+    <t>Manager is required.</t>
+  </si>
+  <si>
+    <t>Validate errors on User's Office</t>
+  </si>
+  <si>
+    <t>Validate errors on User's Manager</t>
+  </si>
+  <si>
+    <t>This email address is assigned to some other user, please update accordingly.</t>
+  </si>
+  <si>
+    <t>hmouloud10@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1065,6 +1129,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1092,7 +1190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1115,11 +1213,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1141,8 +1251,28 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1421,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B498BF-A8CF-47F6-ABEC-D170371E774D}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1436,7 +1566,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>285</v>
@@ -1456,7 +1586,7 @@
         <v>290</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D2" s="1" t="b">
         <v>1</v>
@@ -1470,7 +1600,7 @@
         <v>291</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>1</v>
@@ -1484,7 +1614,7 @@
         <v>288</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D4" s="1" t="b">
         <v>1</v>
@@ -1498,7 +1628,7 @@
         <v>292</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D5" s="1" t="b">
         <v>1</v>
@@ -1512,10 +1642,10 @@
         <v>293</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1526,7 +1656,7 @@
         <v>294</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D7" s="1" t="b">
         <v>1</v>
@@ -1540,15 +1670,43 @@
         <v>295</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D8" s="1" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8" xr:uid="{89FDC481-73BE-4859-A3C9-6AD695471493}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10" xr:uid="{89FDC481-73BE-4859-A3C9-6AD695471493}">
       <formula1>tf</formula1>
     </dataValidation>
   </dataValidations>
@@ -1558,24 +1716,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E063A7-C321-498C-AB7A-8B921DAD62CB}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="33.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="66.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="83.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>285</v>
@@ -1627,7 +1787,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1635,22 +1795,24 @@
         <v>290</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+        <v>325</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>300</v>
+      <c r="B6" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
@@ -1660,8 +1822,8 @@
       <c r="B7" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="C7" s="11">
-        <v>1234</v>
+      <c r="C7" s="11" t="s">
+        <v>301</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>300</v>
@@ -1674,12 +1836,14 @@
       <c r="B8" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="11">
+        <v>1234</v>
+      </c>
       <c r="D8" s="12" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1687,34 +1851,36 @@
         <v>291</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="D9" s="10"/>
+        <v>326</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B10" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="9" t="s">
-        <v>307</v>
+      <c r="B11" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
@@ -1725,10 +1891,10 @@
         <v>288</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
@@ -1738,159 +1904,173 @@
       <c r="B13" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="D13" s="9"/>
+      <c r="C13" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="D14" s="14"/>
+      <c r="B14" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="14" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="9" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="10"/>
+      <c r="B18" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>313</v>
+      <c r="B19" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C20" s="5">
-        <v>5712259421</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>313</v>
+      <c r="B20" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C21" s="5">
-        <v>4654646</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>313</v>
+      <c r="B21" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>313</v>
+      <c r="B22" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="D23" s="9"/>
+      <c r="B23" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="14" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B24" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="9" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="C25" s="6">
-        <v>5712259421</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>314</v>
+      <c r="B25" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
@@ -1898,13 +2078,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="C26" s="6">
-        <v>4654646</v>
+        <v>294</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>311</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
@@ -1912,30 +2092,188 @@
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>316</v>
+        <v>294</v>
+      </c>
+      <c r="C27" s="6">
+        <v>5712259421</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C28" s="6">
+        <v>4654646</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C31" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="C32" s="5">
+        <v>5712259421</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="C33" s="5">
+        <v>4654646</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="D28" s="13"/>
+      <c r="D34" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C37" s="24"/>
+      <c r="D37" s="23" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25" t="s">
+        <v>341</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C18" r:id="rId1" xr:uid="{458C8F38-BA53-4AE1-9BF0-759BF8DEBA74}"/>
+    <hyperlink ref="C13" r:id="rId2" display="David.Roberts@militsdev.onmicrosoft.com" xr:uid="{1563E597-5085-4335-B9EF-B3D35E91BC97}"/>
+    <hyperlink ref="C14" r:id="rId3" xr:uid="{66C17447-D80F-48C4-8548-23B033CDA41B}"/>
+    <hyperlink ref="C16" r:id="rId4" xr:uid="{0826882C-8F65-46F0-9C73-7ACC35C3CD3E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>